<commit_message>
add the possibility to calibrate spatial disaggregation on LAD level with electricity demand data
</commit_message>
<xml_diff>
--- a/energy_demand/config_data/05-technologies/efficiency_generation_spreadsheet.xlsx
+++ b/energy_demand/config_data/05-technologies/efficiency_generation_spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="14460" windowHeight="14925" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="14460" windowHeight="14925"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1849,7 +1849,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1985,6 +1985,8 @@
     <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="93" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="141">
     <cellStyle name="%" xfId="42"/>
@@ -3339,10 +3341,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3359,12 +3361,12 @@
     <col min="10" max="10" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" s="10" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="11" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -3396,1302 +3398,1255 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="100">
         <v>2.9282576866764276E-2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="100">
         <v>3.3674963396778917E-2</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="99">
         <v>2050</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="99">
         <v>2000</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="15">
-        <v>1</v>
-      </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="15" t="s">
+      <c r="I4" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="99" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="100">
         <v>3.6603221083455345E-2</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="100">
         <v>7.320644216691069E-2</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="99">
         <v>2050</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="99">
         <v>2000</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="I5" s="15">
-        <v>1</v>
-      </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="I5" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="100">
         <v>0.21961932650073207</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="100">
         <v>0.29282576866764276</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="99">
         <v>2050</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="99">
         <v>2000</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="15">
-        <v>1</v>
-      </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="I6" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="100">
         <v>0.14641288433382138</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="100">
         <v>0.21961932650073207</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="99">
         <v>2050</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="99">
         <v>2000</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="15">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="I7" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="100">
         <v>0.21961932650073207</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="100">
         <v>0.43923865300146414</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="99">
         <v>2050</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="99">
         <v>2000</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="15">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="I8" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="7">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="C9" s="100">
+        <v>1</v>
+      </c>
+      <c r="D9" s="100">
         <v>1.3336363059657026</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="99">
         <v>2050</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="99">
         <v>2000</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="31">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="I9" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="7">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="C10" s="100">
+        <v>1</v>
+      </c>
+      <c r="D10" s="100">
         <v>3.0759063048538628</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="99">
         <v>2050</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="99">
         <v>2000</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="31">
-        <v>1</v>
-      </c>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="I10" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="7">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
+      <c r="C11" s="100">
+        <v>1</v>
+      </c>
+      <c r="D11" s="100">
         <v>1.3670858320416253</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="99">
         <v>2050</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="99">
         <v>2000</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="31">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="I11" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7">
+      <c r="C12" s="100">
+        <v>1</v>
+      </c>
+      <c r="D12" s="100">
         <v>1.3336363059657026</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="99">
         <v>2050</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="99">
         <v>2000</v>
       </c>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="31">
-        <v>1</v>
-      </c>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="I12" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="100">
         <v>0.4</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="100">
         <v>0.5</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="99">
         <v>2050</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="99">
         <v>2000</v>
       </c>
-      <c r="H13" s="31" t="s">
+      <c r="H13" s="99" t="s">
         <v>133</v>
       </c>
-      <c r="I13" s="31">
-        <v>1</v>
-      </c>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="I13" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="100">
         <v>0.6</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="100">
         <v>0.7</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="99">
         <v>2050</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="99">
         <v>2000</v>
       </c>
-      <c r="H14" s="31" t="s">
+      <c r="H14" s="99" t="s">
         <v>133</v>
       </c>
-      <c r="I14" s="31">
-        <v>1</v>
-      </c>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="I14" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="100">
         <v>0.75</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="100">
         <v>0.9</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="99">
         <v>2050</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="99">
         <v>2000</v>
       </c>
-      <c r="H15" s="31" t="s">
+      <c r="H15" s="99" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="31">
-        <v>1</v>
-      </c>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="I15" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="100">
         <v>0.4</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="100">
         <v>0.5</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="99">
         <v>2050</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="99">
         <v>2000</v>
       </c>
-      <c r="H16" s="31" t="s">
+      <c r="H16" s="99" t="s">
         <v>133</v>
       </c>
-      <c r="I16" s="31">
-        <v>1</v>
-      </c>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="I16" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="100">
         <v>0.4</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="100">
         <v>0.5</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="99">
         <v>2050</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="99">
         <v>2000</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="99" t="s">
         <v>133</v>
       </c>
-      <c r="I17" s="31">
-        <v>1</v>
-      </c>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="I17" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="7">
-        <v>1</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="C18" s="100">
+        <v>1</v>
+      </c>
+      <c r="D18" s="100">
         <v>2.708983419751144</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="99">
         <v>2050</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="99">
         <v>2000</v>
       </c>
-      <c r="H18" s="31" t="s">
+      <c r="H18" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="I18" s="31">
-        <v>1</v>
-      </c>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="I18" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="7">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7">
+      <c r="C19" s="100">
+        <v>1</v>
+      </c>
+      <c r="D19" s="100">
         <v>2.4053173378702097</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="99">
         <v>2050</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="31">
+      <c r="G19" s="99">
         <v>2000</v>
       </c>
-      <c r="H19" s="31" t="s">
+      <c r="H19" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="I19" s="31">
-        <v>1</v>
-      </c>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="I19" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="7">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7">
+      <c r="C20" s="100">
+        <v>1</v>
+      </c>
+      <c r="D20" s="100">
         <v>2.4077602376407699</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="99">
         <v>2050</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="31">
+      <c r="G20" s="99">
         <v>2000</v>
       </c>
-      <c r="H20" s="31" t="s">
+      <c r="H20" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="I20" s="31">
-        <v>1</v>
-      </c>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="I20" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="7">
-        <v>1</v>
-      </c>
-      <c r="D21" s="7">
+      <c r="C21" s="100">
+        <v>1</v>
+      </c>
+      <c r="D21" s="100">
         <v>2.4999611715788794</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="99">
         <v>2050</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="31">
+      <c r="G21" s="99">
         <v>2000</v>
       </c>
-      <c r="H21" s="31" t="s">
+      <c r="H21" s="99" t="s">
         <v>187</v>
       </c>
-      <c r="I21" s="31">
-        <v>1</v>
-      </c>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="I21" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="7">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7">
+      <c r="C22" s="100">
+        <v>1</v>
+      </c>
+      <c r="D22" s="100">
         <v>2</v>
       </c>
-      <c r="E22" s="73">
+      <c r="E22" s="99">
         <v>2050</v>
       </c>
-      <c r="F22" s="73" t="s">
+      <c r="F22" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="73">
+      <c r="G22" s="99">
         <v>2000</v>
       </c>
-      <c r="H22" s="73" t="s">
+      <c r="H22" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="I22" s="73">
-        <v>1</v>
-      </c>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="73" t="s">
+      <c r="I22" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="99" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="7">
-        <v>1</v>
-      </c>
-      <c r="D23" s="7">
+      <c r="C23" s="100">
+        <v>1</v>
+      </c>
+      <c r="D23" s="100">
         <v>2</v>
       </c>
-      <c r="E23" s="73">
+      <c r="E23" s="99">
         <v>2050</v>
       </c>
-      <c r="F23" s="73" t="s">
+      <c r="F23" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="73">
+      <c r="G23" s="99">
         <v>2000</v>
       </c>
-      <c r="H23" s="73" t="s">
+      <c r="H23" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="I23" s="73">
-        <v>1</v>
-      </c>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="s">
+      <c r="I23" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="73" t="s">
+      <c r="B24" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="7">
-        <v>1</v>
-      </c>
-      <c r="D24" s="7">
+      <c r="C24" s="100">
+        <v>1</v>
+      </c>
+      <c r="D24" s="100">
         <v>2</v>
       </c>
-      <c r="E24" s="73">
+      <c r="E24" s="99">
         <v>2050</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="73">
+      <c r="G24" s="99">
         <v>2000</v>
       </c>
-      <c r="H24" s="73" t="s">
+      <c r="H24" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="I24" s="73">
-        <v>1</v>
-      </c>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="73" t="s">
+      <c r="I24" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="73" t="s">
+      <c r="B25" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="7">
-        <v>1</v>
-      </c>
-      <c r="D25" s="7">
+      <c r="C25" s="100">
+        <v>1</v>
+      </c>
+      <c r="D25" s="100">
         <v>2</v>
       </c>
-      <c r="E25" s="73">
+      <c r="E25" s="99">
         <v>2050</v>
       </c>
-      <c r="F25" s="73" t="s">
+      <c r="F25" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="73">
+      <c r="G25" s="99">
         <v>2000</v>
       </c>
-      <c r="H25" s="73" t="s">
+      <c r="H25" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="I25" s="73">
-        <v>1</v>
-      </c>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="73" t="s">
+      <c r="I25" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="73" t="s">
+      <c r="B26" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="C26" s="7">
-        <v>1</v>
-      </c>
-      <c r="D26" s="7">
+      <c r="C26" s="100">
+        <v>1</v>
+      </c>
+      <c r="D26" s="100">
         <v>2</v>
       </c>
-      <c r="E26" s="73">
+      <c r="E26" s="99">
         <v>2050</v>
       </c>
-      <c r="F26" s="73" t="s">
+      <c r="F26" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="73">
+      <c r="G26" s="99">
         <v>2000</v>
       </c>
-      <c r="H26" s="73" t="s">
+      <c r="H26" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="I26" s="73">
+      <c r="I26" s="99">
         <v>0.89</v>
       </c>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="73" t="s">
+    </row>
+    <row r="27" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="73" t="s">
+      <c r="B27" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="7">
-        <v>1</v>
-      </c>
-      <c r="D27" s="7">
+      <c r="C27" s="100">
+        <v>1</v>
+      </c>
+      <c r="D27" s="100">
         <v>2</v>
       </c>
-      <c r="E27" s="73">
+      <c r="E27" s="99">
         <v>2050</v>
       </c>
-      <c r="F27" s="73" t="s">
+      <c r="F27" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="73">
+      <c r="G27" s="99">
         <v>2000</v>
       </c>
-      <c r="H27" s="73" t="s">
+      <c r="H27" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="I27" s="73">
+      <c r="I27" s="99">
         <v>0.89</v>
       </c>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="73" t="s">
+    </row>
+    <row r="28" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="92" t="s">
+      <c r="B28" s="99" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="100">
         <v>0.6</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="100">
         <v>0.7</v>
       </c>
-      <c r="E28" s="92">
+      <c r="E28" s="99">
         <v>2050</v>
       </c>
-      <c r="F28" s="92" t="s">
+      <c r="F28" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G28" s="92">
+      <c r="G28" s="99">
         <v>2000</v>
       </c>
-      <c r="H28" s="92" t="s">
+      <c r="H28" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="I28" s="92">
-        <v>1</v>
-      </c>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="92" t="s">
+      <c r="I28" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="92" t="s">
+      <c r="B29" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="100">
         <v>0.65</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="100">
         <v>0.94</v>
       </c>
-      <c r="E29" s="92">
+      <c r="E29" s="99">
         <v>2050</v>
       </c>
-      <c r="F29" s="92" t="s">
+      <c r="F29" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="92">
+      <c r="G29" s="99">
         <v>2000</v>
       </c>
-      <c r="H29" s="92" t="s">
+      <c r="H29" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="I29" s="92">
+      <c r="I29" s="99">
         <v>0.89</v>
       </c>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="92" t="s">
+    </row>
+    <row r="30" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="92" t="s">
+      <c r="B30" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="100">
         <v>0.99</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="100">
         <v>0.99</v>
       </c>
-      <c r="E30" s="92">
+      <c r="E30" s="99">
         <v>2050</v>
       </c>
-      <c r="F30" s="92" t="s">
+      <c r="F30" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="92">
+      <c r="G30" s="99">
         <v>2000</v>
       </c>
-      <c r="H30" s="92" t="s">
+      <c r="H30" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="I30" s="92">
-        <v>1</v>
-      </c>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="92" t="s">
+      <c r="I30" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="92" t="s">
+      <c r="B31" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="100">
         <v>0.7</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="100">
         <v>0.94</v>
       </c>
-      <c r="E31" s="92">
+      <c r="E31" s="99">
         <v>2050</v>
       </c>
-      <c r="F31" s="92" t="s">
+      <c r="F31" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G31" s="92">
+      <c r="G31" s="99">
         <v>2000</v>
       </c>
-      <c r="H31" s="92" t="s">
+      <c r="H31" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="I31" s="92">
-        <v>1</v>
-      </c>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="92" t="s">
+      <c r="I31" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="92" t="s">
+      <c r="B32" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="100">
         <v>0.6</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="100">
         <v>0.95</v>
       </c>
-      <c r="E32" s="92">
+      <c r="E32" s="99">
         <v>2050</v>
       </c>
-      <c r="F32" s="92" t="s">
+      <c r="F32" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="92">
+      <c r="G32" s="99">
         <v>2000</v>
       </c>
-      <c r="H32" s="92" t="s">
+      <c r="H32" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="I32" s="92">
-        <v>1</v>
-      </c>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="92" t="s">
+      <c r="I32" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="92" t="s">
+      <c r="B33" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="100">
         <v>0.85</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="100">
         <v>0.95</v>
       </c>
-      <c r="E33" s="92">
+      <c r="E33" s="99">
         <v>2050</v>
       </c>
-      <c r="F33" s="92" t="s">
+      <c r="F33" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G33" s="92">
+      <c r="G33" s="99">
         <v>2000</v>
       </c>
-      <c r="H33" s="92" t="s">
+      <c r="H33" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="I33" s="92">
+      <c r="I33" s="99">
         <v>0.89</v>
       </c>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="92" t="s">
+    </row>
+    <row r="34" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="92" t="s">
+      <c r="B34" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="100">
         <v>0.85</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="100">
         <v>0.95</v>
       </c>
-      <c r="E34" s="92">
+      <c r="E34" s="99">
         <v>2050</v>
       </c>
-      <c r="F34" s="92" t="s">
+      <c r="F34" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="92">
+      <c r="G34" s="99">
         <v>2000</v>
       </c>
-      <c r="H34" s="92" t="s">
+      <c r="H34" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="I34" s="92">
-        <v>1</v>
-      </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="92" t="s">
+      <c r="I34" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="92" t="s">
+      <c r="B35" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="100">
         <v>0.85</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="100">
         <v>0.95</v>
       </c>
-      <c r="E35" s="92">
+      <c r="E35" s="99">
         <v>2050</v>
       </c>
-      <c r="F35" s="92" t="s">
+      <c r="F35" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G35" s="92">
+      <c r="G35" s="99">
         <v>2000</v>
       </c>
-      <c r="H35" s="92" t="s">
+      <c r="H35" s="99" t="s">
         <v>156</v>
       </c>
-      <c r="I35" s="92">
-        <v>1</v>
-      </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="92" t="s">
+      <c r="I35" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="92" t="s">
+      <c r="B36" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="100">
         <v>0.8</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="100">
         <v>0.95</v>
       </c>
-      <c r="E36" s="92">
+      <c r="E36" s="99">
         <v>2050</v>
       </c>
-      <c r="F36" s="92" t="s">
+      <c r="F36" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G36" s="92">
+      <c r="G36" s="99">
         <v>2000</v>
       </c>
-      <c r="H36" s="92" t="s">
+      <c r="H36" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="I36" s="92">
+      <c r="I36" s="99">
         <v>0.89</v>
       </c>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="92" t="s">
+    </row>
+    <row r="37" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="92" t="s">
+      <c r="B37" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="100">
         <v>0.85</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="100">
         <v>0.95</v>
       </c>
-      <c r="E37" s="92">
+      <c r="E37" s="99">
         <v>2050</v>
       </c>
-      <c r="F37" s="92" t="s">
+      <c r="F37" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G37" s="92">
+      <c r="G37" s="99">
         <v>2000</v>
       </c>
-      <c r="H37" s="92" t="s">
+      <c r="H37" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="I37" s="92">
+      <c r="I37" s="99">
         <v>0.89</v>
       </c>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="92" t="s">
+    </row>
+    <row r="38" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="92" t="s">
+      <c r="B38" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="100">
         <v>0.99</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="100">
         <v>0.99</v>
       </c>
-      <c r="E38" s="92">
+      <c r="E38" s="99">
         <v>2050</v>
       </c>
-      <c r="F38" s="92" t="s">
+      <c r="F38" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G38" s="92">
+      <c r="G38" s="99">
         <v>2000</v>
       </c>
-      <c r="H38" s="92" t="s">
+      <c r="H38" s="99" t="s">
         <v>158</v>
       </c>
-      <c r="I38" s="92">
-        <v>1</v>
-      </c>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="92" t="s">
+      <c r="I38" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="92" t="s">
+      <c r="B39" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="100">
         <v>0.99</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="100">
         <v>0.99</v>
       </c>
-      <c r="E39" s="92">
+      <c r="E39" s="99">
         <v>2050</v>
       </c>
-      <c r="F39" s="92" t="s">
+      <c r="F39" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G39" s="92">
+      <c r="G39" s="99">
         <v>2000</v>
       </c>
-      <c r="H39" s="92" t="s">
+      <c r="H39" s="99" t="s">
         <v>159</v>
       </c>
-      <c r="I39" s="92">
-        <v>1</v>
-      </c>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="92" t="s">
+      <c r="I39" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="92" t="s">
+      <c r="B40" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="100">
         <v>3.6</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="100">
         <v>4</v>
       </c>
-      <c r="E40" s="92">
+      <c r="E40" s="99">
         <v>2050</v>
       </c>
-      <c r="F40" s="92" t="s">
+      <c r="F40" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G40" s="92">
+      <c r="G40" s="99">
         <v>2000</v>
       </c>
-      <c r="H40" s="92" t="s">
+      <c r="H40" s="99" t="s">
         <v>160</v>
       </c>
-      <c r="I40" s="92">
-        <v>1</v>
-      </c>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="92" t="s">
+      <c r="I40" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="92" t="s">
+      <c r="B41" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="100">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="100">
         <v>5.4</v>
       </c>
-      <c r="E41" s="92">
+      <c r="E41" s="99">
         <v>2050</v>
       </c>
-      <c r="F41" s="92" t="s">
+      <c r="F41" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G41" s="92">
+      <c r="G41" s="99">
         <v>2000</v>
       </c>
-      <c r="H41" s="92" t="s">
+      <c r="H41" s="99" t="s">
         <v>160</v>
       </c>
-      <c r="I41" s="92">
-        <v>1</v>
-      </c>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="92" t="s">
+      <c r="I41" s="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="92" t="s">
+      <c r="B42" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="100">
         <v>3.6</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="100">
         <v>4</v>
       </c>
-      <c r="E42" s="92">
+      <c r="E42" s="99">
         <v>2050</v>
       </c>
-      <c r="F42" s="92" t="s">
+      <c r="F42" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="92">
+      <c r="G42" s="99">
         <v>2000</v>
       </c>
-      <c r="H42" s="92" t="s">
+      <c r="H42" s="99" t="s">
         <v>160</v>
       </c>
-      <c r="I42" s="92">
+      <c r="I42" s="99">
         <v>0.89</v>
       </c>
-      <c r="J42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="92" t="s">
+    </row>
+    <row r="43" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="92" t="s">
+      <c r="B43" s="99" t="s">
         <v>128</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="100">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="100">
         <v>5.4</v>
       </c>
-      <c r="E43" s="92">
+      <c r="E43" s="99">
         <v>2050</v>
       </c>
-      <c r="F43" s="92" t="s">
+      <c r="F43" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="92">
+      <c r="G43" s="99">
         <v>2000</v>
       </c>
-      <c r="H43" s="92" t="s">
+      <c r="H43" s="99" t="s">
         <v>160</v>
       </c>
-      <c r="I43" s="92">
+      <c r="I43" s="99">
         <v>0.89</v>
       </c>
-      <c r="J43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="92" t="s">
+    </row>
+    <row r="44" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="92" t="s">
+      <c r="B44" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="100">
         <v>0.45</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="100">
         <v>0.45</v>
       </c>
-      <c r="E44" s="92">
+      <c r="E44" s="99">
         <v>2050</v>
       </c>
-      <c r="F44" s="92" t="s">
+      <c r="F44" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G44" s="92">
+      <c r="G44" s="99">
         <v>2000</v>
       </c>
-      <c r="H44" s="92" t="s">
+      <c r="H44" s="99" t="s">
         <v>157</v>
       </c>
-      <c r="I44" s="92">
+      <c r="I44" s="99">
         <v>0.2</v>
       </c>
-      <c r="J44" s="95" t="s">
+      <c r="J44" s="99" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="92" t="s">
+    <row r="45" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="92" t="s">
+      <c r="B45" s="99" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="7">
-        <v>1</v>
-      </c>
-      <c r="D45" s="7">
-        <v>1</v>
-      </c>
-      <c r="E45" s="92">
+      <c r="C45" s="100">
+        <v>1</v>
+      </c>
+      <c r="D45" s="100">
+        <v>1</v>
+      </c>
+      <c r="E45" s="99">
         <v>2050</v>
       </c>
-      <c r="F45" s="92" t="s">
+      <c r="F45" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="92">
+      <c r="G45" s="99">
         <v>2000</v>
       </c>
-      <c r="H45" s="92" t="s">
+      <c r="H45" s="99" t="s">
         <v>161</v>
       </c>
-      <c r="I45" s="92">
+      <c r="I45" s="99">
         <v>0.2</v>
       </c>
-      <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="92" t="s">
+    </row>
+    <row r="46" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="92" t="s">
+      <c r="B46" s="99" t="s">
         <v>127</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="100">
         <v>0.6</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="100">
         <v>0.6</v>
       </c>
-      <c r="E46" s="92">
+      <c r="E46" s="99">
         <v>2050</v>
       </c>
-      <c r="F46" s="92" t="s">
+      <c r="F46" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="G46" s="92">
+      <c r="G46" s="99">
         <v>2000</v>
       </c>
-      <c r="H46" s="92" t="s">
+      <c r="H46" s="99" t="s">
         <v>161</v>
       </c>
-      <c r="I46" s="92">
+      <c r="I46" s="99">
         <v>0.2</v>
       </c>
-      <c r="J46" s="5"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="92" t="s">
@@ -5237,7 +5192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
@@ -7031,8 +6986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX137"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed efficiency of Electric arc furnace
</commit_message>
<xml_diff>
--- a/energy_demand/config_data/05-technologies/efficiency_generation_spreadsheet.xlsx
+++ b/energy_demand/config_data/05-technologies/efficiency_generation_spreadsheet.xlsx
@@ -1976,6 +1976,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1985,8 +1987,6 @@
     <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="93" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="141">
     <cellStyle name="%" xfId="42"/>
@@ -3343,8 +3343,8 @@
   </sheetPr>
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3398,1253 +3398,1253 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+    <row r="4" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="100">
+      <c r="C4" s="97">
         <v>2.9282576866764276E-2</v>
       </c>
-      <c r="D4" s="100">
+      <c r="D4" s="97">
         <v>3.3674963396778917E-2</v>
       </c>
-      <c r="E4" s="99">
+      <c r="E4" s="96">
         <v>2050</v>
       </c>
-      <c r="F4" s="99" t="s">
+      <c r="F4" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="99">
+      <c r="G4" s="96">
         <v>2000</v>
       </c>
-      <c r="H4" s="99" t="s">
+      <c r="H4" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="99" t="s">
+      <c r="I4" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="100">
+      <c r="C5" s="97">
         <v>3.6603221083455345E-2</v>
       </c>
-      <c r="D5" s="100">
+      <c r="D5" s="97">
         <v>7.320644216691069E-2</v>
       </c>
-      <c r="E5" s="99">
+      <c r="E5" s="96">
         <v>2050</v>
       </c>
-      <c r="F5" s="99" t="s">
+      <c r="F5" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="99">
+      <c r="G5" s="96">
         <v>2000</v>
       </c>
-      <c r="H5" s="99" t="s">
+      <c r="H5" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="I5" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="s">
+      <c r="I5" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="100">
+      <c r="C6" s="97">
         <v>0.21961932650073207</v>
       </c>
-      <c r="D6" s="100">
+      <c r="D6" s="97">
         <v>0.29282576866764276</v>
       </c>
-      <c r="E6" s="99">
+      <c r="E6" s="96">
         <v>2050</v>
       </c>
-      <c r="F6" s="99" t="s">
+      <c r="F6" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="99">
+      <c r="G6" s="96">
         <v>2000</v>
       </c>
-      <c r="H6" s="99" t="s">
+      <c r="H6" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="I6" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="s">
+      <c r="I6" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="99" t="s">
+      <c r="B7" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="100">
+      <c r="C7" s="97">
         <v>0.14641288433382138</v>
       </c>
-      <c r="D7" s="100">
+      <c r="D7" s="97">
         <v>0.21961932650073207</v>
       </c>
-      <c r="E7" s="99">
+      <c r="E7" s="96">
         <v>2050</v>
       </c>
-      <c r="F7" s="99" t="s">
+      <c r="F7" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="99">
+      <c r="G7" s="96">
         <v>2000</v>
       </c>
-      <c r="H7" s="99" t="s">
+      <c r="H7" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="99" t="s">
+      <c r="I7" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="100">
+      <c r="C8" s="97">
         <v>0.21961932650073207</v>
       </c>
-      <c r="D8" s="100">
+      <c r="D8" s="97">
         <v>0.43923865300146414</v>
       </c>
-      <c r="E8" s="99">
+      <c r="E8" s="96">
         <v>2050</v>
       </c>
-      <c r="F8" s="99" t="s">
+      <c r="F8" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="99">
+      <c r="G8" s="96">
         <v>2000</v>
       </c>
-      <c r="H8" s="99" t="s">
+      <c r="H8" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99" t="s">
+      <c r="I8" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="100">
-        <v>1</v>
-      </c>
-      <c r="D9" s="100">
+      <c r="C9" s="97">
+        <v>1</v>
+      </c>
+      <c r="D9" s="97">
         <v>1.3336363059657026</v>
       </c>
-      <c r="E9" s="99">
+      <c r="E9" s="96">
         <v>2050</v>
       </c>
-      <c r="F9" s="99" t="s">
+      <c r="F9" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="99">
+      <c r="G9" s="96">
         <v>2000</v>
       </c>
-      <c r="H9" s="99" t="s">
+      <c r="H9" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="I9" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="99" t="s">
+      <c r="I9" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="99" t="s">
+      <c r="B10" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="100">
-        <v>1</v>
-      </c>
-      <c r="D10" s="100">
+      <c r="C10" s="97">
+        <v>1</v>
+      </c>
+      <c r="D10" s="97">
         <v>3.0759063048538628</v>
       </c>
-      <c r="E10" s="99">
+      <c r="E10" s="96">
         <v>2050</v>
       </c>
-      <c r="F10" s="99" t="s">
+      <c r="F10" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="99">
+      <c r="G10" s="96">
         <v>2000</v>
       </c>
-      <c r="H10" s="99" t="s">
+      <c r="H10" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="99" t="s">
+      <c r="I10" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="100">
-        <v>1</v>
-      </c>
-      <c r="D11" s="100">
+      <c r="C11" s="97">
+        <v>1</v>
+      </c>
+      <c r="D11" s="97">
         <v>1.3670858320416253</v>
       </c>
-      <c r="E11" s="99">
+      <c r="E11" s="96">
         <v>2050</v>
       </c>
-      <c r="F11" s="99" t="s">
+      <c r="F11" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="99">
+      <c r="G11" s="96">
         <v>2000</v>
       </c>
-      <c r="H11" s="99" t="s">
+      <c r="H11" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="99" t="s">
+      <c r="I11" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="100">
-        <v>1</v>
-      </c>
-      <c r="D12" s="100">
+      <c r="C12" s="97">
+        <v>1</v>
+      </c>
+      <c r="D12" s="97">
         <v>1.3336363059657026</v>
       </c>
-      <c r="E12" s="99">
+      <c r="E12" s="96">
         <v>2050</v>
       </c>
-      <c r="F12" s="99" t="s">
+      <c r="F12" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="99">
+      <c r="G12" s="96">
         <v>2000</v>
       </c>
-      <c r="H12" s="99" t="s">
+      <c r="H12" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="99" t="s">
+      <c r="I12" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="99" t="s">
+      <c r="B13" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="100">
+      <c r="C13" s="97">
         <v>0.4</v>
       </c>
-      <c r="D13" s="100">
+      <c r="D13" s="97">
         <v>0.5</v>
       </c>
-      <c r="E13" s="99">
+      <c r="E13" s="96">
         <v>2050</v>
       </c>
-      <c r="F13" s="99" t="s">
+      <c r="F13" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="99">
+      <c r="G13" s="96">
         <v>2000</v>
       </c>
-      <c r="H13" s="99" t="s">
+      <c r="H13" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="I13" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="99" t="s">
+      <c r="I13" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="100">
+      <c r="C14" s="97">
         <v>0.6</v>
       </c>
-      <c r="D14" s="100">
+      <c r="D14" s="97">
         <v>0.7</v>
       </c>
-      <c r="E14" s="99">
+      <c r="E14" s="96">
         <v>2050</v>
       </c>
-      <c r="F14" s="99" t="s">
+      <c r="F14" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="99">
+      <c r="G14" s="96">
         <v>2000</v>
       </c>
-      <c r="H14" s="99" t="s">
+      <c r="H14" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="I14" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="99" t="s">
+      <c r="I14" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="99" t="s">
+      <c r="B15" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C15" s="97">
         <v>0.75</v>
       </c>
-      <c r="D15" s="100">
+      <c r="D15" s="97">
         <v>0.9</v>
       </c>
-      <c r="E15" s="99">
+      <c r="E15" s="96">
         <v>2050</v>
       </c>
-      <c r="F15" s="99" t="s">
+      <c r="F15" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="99">
+      <c r="G15" s="96">
         <v>2000</v>
       </c>
-      <c r="H15" s="99" t="s">
+      <c r="H15" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="I15" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="s">
+      <c r="I15" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="96" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="99" t="s">
+      <c r="B16" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="100">
+      <c r="C16" s="97">
         <v>0.4</v>
       </c>
-      <c r="D16" s="100">
+      <c r="D16" s="97">
         <v>0.5</v>
       </c>
-      <c r="E16" s="99">
+      <c r="E16" s="96">
         <v>2050</v>
       </c>
-      <c r="F16" s="99" t="s">
+      <c r="F16" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="99">
+      <c r="G16" s="96">
         <v>2000</v>
       </c>
-      <c r="H16" s="99" t="s">
+      <c r="H16" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="I16" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="99" t="s">
+      <c r="I16" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="C17" s="100">
+      <c r="C17" s="97">
         <v>0.4</v>
       </c>
-      <c r="D17" s="100">
+      <c r="D17" s="97">
         <v>0.5</v>
       </c>
-      <c r="E17" s="99">
+      <c r="E17" s="96">
         <v>2050</v>
       </c>
-      <c r="F17" s="99" t="s">
+      <c r="F17" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G17" s="99">
+      <c r="G17" s="96">
         <v>2000</v>
       </c>
-      <c r="H17" s="99" t="s">
+      <c r="H17" s="96" t="s">
         <v>133</v>
       </c>
-      <c r="I17" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="99" t="s">
+      <c r="I17" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="99" t="s">
+      <c r="B18" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="100">
-        <v>1</v>
-      </c>
-      <c r="D18" s="100">
+      <c r="C18" s="97">
+        <v>1</v>
+      </c>
+      <c r="D18" s="97">
         <v>2.708983419751144</v>
       </c>
-      <c r="E18" s="99">
+      <c r="E18" s="96">
         <v>2050</v>
       </c>
-      <c r="F18" s="99" t="s">
+      <c r="F18" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="99">
+      <c r="G18" s="96">
         <v>2000</v>
       </c>
-      <c r="H18" s="99" t="s">
+      <c r="H18" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="I18" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="99" t="s">
+      <c r="I18" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="99" t="s">
+      <c r="B19" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="100">
-        <v>1</v>
-      </c>
-      <c r="D19" s="100">
+      <c r="C19" s="97">
+        <v>1</v>
+      </c>
+      <c r="D19" s="97">
         <v>2.4053173378702097</v>
       </c>
-      <c r="E19" s="99">
+      <c r="E19" s="96">
         <v>2050</v>
       </c>
-      <c r="F19" s="99" t="s">
+      <c r="F19" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="99">
+      <c r="G19" s="96">
         <v>2000</v>
       </c>
-      <c r="H19" s="99" t="s">
+      <c r="H19" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="I19" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="99" t="s">
+      <c r="I19" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="99" t="s">
+      <c r="B20" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="100">
-        <v>1</v>
-      </c>
-      <c r="D20" s="100">
+      <c r="C20" s="97">
+        <v>1</v>
+      </c>
+      <c r="D20" s="97">
         <v>2.4077602376407699</v>
       </c>
-      <c r="E20" s="99">
+      <c r="E20" s="96">
         <v>2050</v>
       </c>
-      <c r="F20" s="99" t="s">
+      <c r="F20" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="99">
+      <c r="G20" s="96">
         <v>2000</v>
       </c>
-      <c r="H20" s="99" t="s">
+      <c r="H20" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="I20" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="99" t="s">
+      <c r="I20" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="99" t="s">
+      <c r="B21" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="100">
-        <v>1</v>
-      </c>
-      <c r="D21" s="100">
+      <c r="C21" s="97">
+        <v>1</v>
+      </c>
+      <c r="D21" s="97">
         <v>2.4999611715788794</v>
       </c>
-      <c r="E21" s="99">
+      <c r="E21" s="96">
         <v>2050</v>
       </c>
-      <c r="F21" s="99" t="s">
+      <c r="F21" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="99">
+      <c r="G21" s="96">
         <v>2000</v>
       </c>
-      <c r="H21" s="99" t="s">
+      <c r="H21" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="I21" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="99" t="s">
+      <c r="I21" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="100">
-        <v>1</v>
-      </c>
-      <c r="D22" s="100">
+      <c r="C22" s="97">
+        <v>1</v>
+      </c>
+      <c r="D22" s="97">
         <v>2</v>
       </c>
-      <c r="E22" s="99">
+      <c r="E22" s="96">
         <v>2050</v>
       </c>
-      <c r="F22" s="99" t="s">
+      <c r="F22" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="99">
+      <c r="G22" s="96">
         <v>2000</v>
       </c>
-      <c r="H22" s="99" t="s">
+      <c r="H22" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="I22" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="99" t="s">
+      <c r="I22" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="99" t="s">
+      <c r="B23" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="100">
-        <v>1</v>
-      </c>
-      <c r="D23" s="100">
+      <c r="C23" s="97">
+        <v>1</v>
+      </c>
+      <c r="D23" s="97">
         <v>2</v>
       </c>
-      <c r="E23" s="99">
+      <c r="E23" s="96">
         <v>2050</v>
       </c>
-      <c r="F23" s="99" t="s">
+      <c r="F23" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G23" s="99">
+      <c r="G23" s="96">
         <v>2000</v>
       </c>
-      <c r="H23" s="99" t="s">
+      <c r="H23" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="I23" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="99" t="s">
+      <c r="I23" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="99" t="s">
+      <c r="B24" s="96" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="100">
-        <v>1</v>
-      </c>
-      <c r="D24" s="100">
+      <c r="C24" s="97">
+        <v>1</v>
+      </c>
+      <c r="D24" s="97">
         <v>2</v>
       </c>
-      <c r="E24" s="99">
+      <c r="E24" s="96">
         <v>2050</v>
       </c>
-      <c r="F24" s="99" t="s">
+      <c r="F24" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G24" s="99">
+      <c r="G24" s="96">
         <v>2000</v>
       </c>
-      <c r="H24" s="99" t="s">
+      <c r="H24" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="I24" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="99" t="s">
+      <c r="I24" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="99" t="s">
+      <c r="B25" s="96" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="100">
-        <v>1</v>
-      </c>
-      <c r="D25" s="100">
+      <c r="C25" s="97">
+        <v>1</v>
+      </c>
+      <c r="D25" s="97">
         <v>2</v>
       </c>
-      <c r="E25" s="99">
+      <c r="E25" s="96">
         <v>2050</v>
       </c>
-      <c r="F25" s="99" t="s">
+      <c r="F25" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="99">
+      <c r="G25" s="96">
         <v>2000</v>
       </c>
-      <c r="H25" s="99" t="s">
+      <c r="H25" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="I25" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="99" t="s">
+      <c r="I25" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="99" t="s">
+      <c r="B26" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="C26" s="100">
-        <v>1</v>
-      </c>
-      <c r="D26" s="100">
+      <c r="C26" s="97">
+        <v>1</v>
+      </c>
+      <c r="D26" s="97">
         <v>2</v>
       </c>
-      <c r="E26" s="99">
+      <c r="E26" s="96">
         <v>2050</v>
       </c>
-      <c r="F26" s="99" t="s">
+      <c r="F26" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G26" s="99">
+      <c r="G26" s="96">
         <v>2000</v>
       </c>
-      <c r="H26" s="99" t="s">
+      <c r="H26" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="I26" s="99">
+      <c r="I26" s="96">
         <v>0.89</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="99" t="s">
+    <row r="27" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="99" t="s">
+      <c r="B27" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="C27" s="100">
-        <v>1</v>
-      </c>
-      <c r="D27" s="100">
+      <c r="C27" s="97">
+        <v>1</v>
+      </c>
+      <c r="D27" s="97">
         <v>2</v>
       </c>
-      <c r="E27" s="99">
+      <c r="E27" s="96">
         <v>2050</v>
       </c>
-      <c r="F27" s="99" t="s">
+      <c r="F27" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G27" s="99">
+      <c r="G27" s="96">
         <v>2000</v>
       </c>
-      <c r="H27" s="99" t="s">
+      <c r="H27" s="96" t="s">
         <v>141</v>
       </c>
-      <c r="I27" s="99">
+      <c r="I27" s="96">
         <v>0.89</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="99" t="s">
+    <row r="28" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="99" t="s">
+      <c r="B28" s="96" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="100">
+      <c r="C28" s="97">
         <v>0.6</v>
       </c>
-      <c r="D28" s="100">
+      <c r="D28" s="97">
         <v>0.7</v>
       </c>
-      <c r="E28" s="99">
+      <c r="E28" s="96">
         <v>2050</v>
       </c>
-      <c r="F28" s="99" t="s">
+      <c r="F28" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G28" s="99">
+      <c r="G28" s="96">
         <v>2000</v>
       </c>
-      <c r="H28" s="99" t="s">
+      <c r="H28" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="I28" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="99" t="s">
+      <c r="I28" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="99" t="s">
+      <c r="B29" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="100">
+      <c r="C29" s="97">
         <v>0.65</v>
       </c>
-      <c r="D29" s="100">
+      <c r="D29" s="97">
         <v>0.94</v>
       </c>
-      <c r="E29" s="99">
+      <c r="E29" s="96">
         <v>2050</v>
       </c>
-      <c r="F29" s="99" t="s">
+      <c r="F29" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="99">
+      <c r="G29" s="96">
         <v>2000</v>
       </c>
-      <c r="H29" s="99" t="s">
+      <c r="H29" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="I29" s="99">
+      <c r="I29" s="96">
         <v>0.89</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="99" t="s">
+    <row r="30" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="99" t="s">
+      <c r="B30" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C30" s="100">
+      <c r="C30" s="97">
         <v>0.99</v>
       </c>
-      <c r="D30" s="100">
+      <c r="D30" s="97">
         <v>0.99</v>
       </c>
-      <c r="E30" s="99">
+      <c r="E30" s="96">
         <v>2050</v>
       </c>
-      <c r="F30" s="99" t="s">
+      <c r="F30" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G30" s="99">
+      <c r="G30" s="96">
         <v>2000</v>
       </c>
-      <c r="H30" s="99" t="s">
+      <c r="H30" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="I30" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="99" t="s">
+      <c r="I30" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="99" t="s">
+      <c r="B31" s="96" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="100">
+      <c r="C31" s="97">
         <v>0.7</v>
       </c>
-      <c r="D31" s="100">
+      <c r="D31" s="97">
         <v>0.94</v>
       </c>
-      <c r="E31" s="99">
+      <c r="E31" s="96">
         <v>2050</v>
       </c>
-      <c r="F31" s="99" t="s">
+      <c r="F31" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G31" s="99">
+      <c r="G31" s="96">
         <v>2000</v>
       </c>
-      <c r="H31" s="99" t="s">
+      <c r="H31" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="I31" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="99" t="s">
+      <c r="I31" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="99" t="s">
+      <c r="B32" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="100">
+      <c r="C32" s="97">
         <v>0.6</v>
       </c>
-      <c r="D32" s="100">
+      <c r="D32" s="97">
         <v>0.95</v>
       </c>
-      <c r="E32" s="99">
+      <c r="E32" s="96">
         <v>2050</v>
       </c>
-      <c r="F32" s="99" t="s">
+      <c r="F32" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G32" s="99">
+      <c r="G32" s="96">
         <v>2000</v>
       </c>
-      <c r="H32" s="99" t="s">
+      <c r="H32" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="I32" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="99" t="s">
+      <c r="I32" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="99" t="s">
+      <c r="B33" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="C33" s="100">
+      <c r="C33" s="97">
         <v>0.85</v>
       </c>
-      <c r="D33" s="100">
+      <c r="D33" s="97">
         <v>0.95</v>
       </c>
-      <c r="E33" s="99">
+      <c r="E33" s="96">
         <v>2050</v>
       </c>
-      <c r="F33" s="99" t="s">
+      <c r="F33" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G33" s="99">
+      <c r="G33" s="96">
         <v>2000</v>
       </c>
-      <c r="H33" s="99" t="s">
+      <c r="H33" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="I33" s="99">
+      <c r="I33" s="96">
         <v>0.89</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="99" t="s">
+    <row r="34" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="99" t="s">
+      <c r="B34" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="100">
+      <c r="C34" s="97">
         <v>0.85</v>
       </c>
-      <c r="D34" s="100">
+      <c r="D34" s="97">
         <v>0.95</v>
       </c>
-      <c r="E34" s="99">
+      <c r="E34" s="96">
         <v>2050</v>
       </c>
-      <c r="F34" s="99" t="s">
+      <c r="F34" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="99">
+      <c r="G34" s="96">
         <v>2000</v>
       </c>
-      <c r="H34" s="99" t="s">
+      <c r="H34" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="I34" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="99" t="s">
+      <c r="I34" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="99" t="s">
+      <c r="B35" s="96" t="s">
         <v>140</v>
       </c>
-      <c r="C35" s="100">
+      <c r="C35" s="97">
         <v>0.85</v>
       </c>
-      <c r="D35" s="100">
+      <c r="D35" s="97">
         <v>0.95</v>
       </c>
-      <c r="E35" s="99">
+      <c r="E35" s="96">
         <v>2050</v>
       </c>
-      <c r="F35" s="99" t="s">
+      <c r="F35" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G35" s="99">
+      <c r="G35" s="96">
         <v>2000</v>
       </c>
-      <c r="H35" s="99" t="s">
+      <c r="H35" s="96" t="s">
         <v>156</v>
       </c>
-      <c r="I35" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="99" t="s">
+      <c r="I35" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="99" t="s">
+      <c r="B36" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="100">
+      <c r="C36" s="97">
         <v>0.8</v>
       </c>
-      <c r="D36" s="100">
+      <c r="D36" s="97">
         <v>0.95</v>
       </c>
-      <c r="E36" s="99">
+      <c r="E36" s="96">
         <v>2050</v>
       </c>
-      <c r="F36" s="99" t="s">
+      <c r="F36" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G36" s="99">
+      <c r="G36" s="96">
         <v>2000</v>
       </c>
-      <c r="H36" s="99" t="s">
+      <c r="H36" s="96" t="s">
         <v>157</v>
       </c>
-      <c r="I36" s="99">
+      <c r="I36" s="96">
         <v>0.89</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="99" t="s">
+    <row r="37" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="99" t="s">
+      <c r="B37" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="100">
+      <c r="C37" s="97">
         <v>0.85</v>
       </c>
-      <c r="D37" s="100">
+      <c r="D37" s="97">
         <v>0.95</v>
       </c>
-      <c r="E37" s="99">
+      <c r="E37" s="96">
         <v>2050</v>
       </c>
-      <c r="F37" s="99" t="s">
+      <c r="F37" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G37" s="99">
+      <c r="G37" s="96">
         <v>2000</v>
       </c>
-      <c r="H37" s="99" t="s">
+      <c r="H37" s="96" t="s">
         <v>157</v>
       </c>
-      <c r="I37" s="99">
+      <c r="I37" s="96">
         <v>0.89</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="99" t="s">
+    <row r="38" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="99" t="s">
+      <c r="B38" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="100">
+      <c r="C38" s="97">
         <v>0.99</v>
       </c>
-      <c r="D38" s="100">
+      <c r="D38" s="97">
         <v>0.99</v>
       </c>
-      <c r="E38" s="99">
+      <c r="E38" s="96">
         <v>2050</v>
       </c>
-      <c r="F38" s="99" t="s">
+      <c r="F38" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G38" s="99">
+      <c r="G38" s="96">
         <v>2000</v>
       </c>
-      <c r="H38" s="99" t="s">
+      <c r="H38" s="96" t="s">
         <v>158</v>
       </c>
-      <c r="I38" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="99" t="s">
+      <c r="I38" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="B39" s="99" t="s">
+      <c r="B39" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C39" s="100">
+      <c r="C39" s="97">
         <v>0.99</v>
       </c>
-      <c r="D39" s="100">
+      <c r="D39" s="97">
         <v>0.99</v>
       </c>
-      <c r="E39" s="99">
+      <c r="E39" s="96">
         <v>2050</v>
       </c>
-      <c r="F39" s="99" t="s">
+      <c r="F39" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G39" s="99">
+      <c r="G39" s="96">
         <v>2000</v>
       </c>
-      <c r="H39" s="99" t="s">
+      <c r="H39" s="96" t="s">
         <v>159</v>
       </c>
-      <c r="I39" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="99" t="s">
+      <c r="I39" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="99" t="s">
+      <c r="B40" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="100">
+      <c r="C40" s="97">
         <v>3.6</v>
       </c>
-      <c r="D40" s="100">
+      <c r="D40" s="97">
         <v>4</v>
       </c>
-      <c r="E40" s="99">
+      <c r="E40" s="96">
         <v>2050</v>
       </c>
-      <c r="F40" s="99" t="s">
+      <c r="F40" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G40" s="99">
+      <c r="G40" s="96">
         <v>2000</v>
       </c>
-      <c r="H40" s="99" t="s">
+      <c r="H40" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="I40" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="99" t="s">
+      <c r="I40" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="99" t="s">
+      <c r="B41" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="100">
+      <c r="C41" s="97">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D41" s="100">
+      <c r="D41" s="97">
         <v>5.4</v>
       </c>
-      <c r="E41" s="99">
+      <c r="E41" s="96">
         <v>2050</v>
       </c>
-      <c r="F41" s="99" t="s">
+      <c r="F41" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G41" s="99">
+      <c r="G41" s="96">
         <v>2000</v>
       </c>
-      <c r="H41" s="99" t="s">
+      <c r="H41" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="I41" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="99" t="s">
+      <c r="I41" s="96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="99" t="s">
+      <c r="B42" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="C42" s="100">
+      <c r="C42" s="97">
         <v>3.6</v>
       </c>
-      <c r="D42" s="100">
+      <c r="D42" s="97">
         <v>4</v>
       </c>
-      <c r="E42" s="99">
+      <c r="E42" s="96">
         <v>2050</v>
       </c>
-      <c r="F42" s="99" t="s">
+      <c r="F42" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="99">
+      <c r="G42" s="96">
         <v>2000</v>
       </c>
-      <c r="H42" s="99" t="s">
+      <c r="H42" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="I42" s="99">
+      <c r="I42" s="96">
         <v>0.89</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="99" t="s">
+    <row r="43" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="99" t="s">
+      <c r="B43" s="96" t="s">
         <v>128</v>
       </c>
-      <c r="C43" s="100">
+      <c r="C43" s="97">
         <v>4.9000000000000004</v>
       </c>
-      <c r="D43" s="100">
+      <c r="D43" s="97">
         <v>5.4</v>
       </c>
-      <c r="E43" s="99">
+      <c r="E43" s="96">
         <v>2050</v>
       </c>
-      <c r="F43" s="99" t="s">
+      <c r="F43" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="99">
+      <c r="G43" s="96">
         <v>2000</v>
       </c>
-      <c r="H43" s="99" t="s">
+      <c r="H43" s="96" t="s">
         <v>160</v>
       </c>
-      <c r="I43" s="99">
+      <c r="I43" s="96">
         <v>0.89</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="99" t="s">
+    <row r="44" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="99" t="s">
+      <c r="B44" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="C44" s="100">
+      <c r="C44" s="97">
         <v>0.45</v>
       </c>
-      <c r="D44" s="100">
+      <c r="D44" s="97">
         <v>0.45</v>
       </c>
-      <c r="E44" s="99">
+      <c r="E44" s="96">
         <v>2050</v>
       </c>
-      <c r="F44" s="99" t="s">
+      <c r="F44" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G44" s="99">
+      <c r="G44" s="96">
         <v>2000</v>
       </c>
-      <c r="H44" s="99" t="s">
+      <c r="H44" s="96" t="s">
         <v>157</v>
       </c>
-      <c r="I44" s="99">
+      <c r="I44" s="96">
         <v>0.2</v>
       </c>
-      <c r="J44" s="99" t="s">
+      <c r="J44" s="96" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="99" t="s">
+    <row r="45" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="99" t="s">
+      <c r="B45" s="96" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="100">
-        <v>1</v>
-      </c>
-      <c r="D45" s="100">
-        <v>1</v>
-      </c>
-      <c r="E45" s="99">
+      <c r="C45" s="97">
+        <v>1</v>
+      </c>
+      <c r="D45" s="97">
+        <v>1</v>
+      </c>
+      <c r="E45" s="96">
         <v>2050</v>
       </c>
-      <c r="F45" s="99" t="s">
+      <c r="F45" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G45" s="99">
+      <c r="G45" s="96">
         <v>2000</v>
       </c>
-      <c r="H45" s="99" t="s">
+      <c r="H45" s="96" t="s">
         <v>161</v>
       </c>
-      <c r="I45" s="99">
+      <c r="I45" s="96">
         <v>0.2</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="99" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="99" t="s">
+    <row r="46" spans="1:10" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="99" t="s">
+      <c r="B46" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="C46" s="100">
+      <c r="C46" s="97">
         <v>0.6</v>
       </c>
-      <c r="D46" s="100">
+      <c r="D46" s="97">
         <v>0.6</v>
       </c>
-      <c r="E46" s="99">
+      <c r="E46" s="96">
         <v>2050</v>
       </c>
-      <c r="F46" s="99" t="s">
+      <c r="F46" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="G46" s="99">
+      <c r="G46" s="96">
         <v>2000</v>
       </c>
-      <c r="H46" s="99" t="s">
+      <c r="H46" s="96" t="s">
         <v>161</v>
       </c>
-      <c r="I46" s="99">
+      <c r="I46" s="96">
         <v>0.2</v>
       </c>
     </row>
@@ -4679,54 +4679,225 @@
       <c r="J47" s="5"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="92"/>
-      <c r="B48" s="92"/>
-      <c r="C48" s="92"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="92"/>
-      <c r="F48" s="92"/>
-      <c r="G48" s="92"/>
-      <c r="H48" s="92"/>
-      <c r="I48" s="92"/>
+      <c r="A48" s="92" t="str">
+        <f>is_high_temp_process!A3:I3</f>
+        <v>basic_oxygen_furnace</v>
+      </c>
+      <c r="B48" s="95" t="str">
+        <f>is_high_temp_process!B3:J3</f>
+        <v>solid_fuel</v>
+      </c>
+      <c r="C48" s="95">
+        <f>is_high_temp_process!C3:K3</f>
+        <v>1</v>
+      </c>
+      <c r="D48" s="95">
+        <f>is_high_temp_process!D3:L3</f>
+        <v>1</v>
+      </c>
+      <c r="E48" s="95">
+        <f>is_high_temp_process!E3:M3</f>
+        <v>2050</v>
+      </c>
+      <c r="F48" s="95" t="str">
+        <f>is_high_temp_process!F3:N3</f>
+        <v>linear</v>
+      </c>
+      <c r="G48" s="95">
+        <f>is_high_temp_process!G3:O3</f>
+        <v>2010</v>
+      </c>
+      <c r="H48" s="95" t="str">
+        <f>is_high_temp_process!H3:P3</f>
+        <v>steel_production</v>
+      </c>
+      <c r="I48" s="95">
+        <f>is_high_temp_process!I3:Q3</f>
+        <v>1</v>
+      </c>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="95" t="str">
+        <f>is_high_temp_process!A4:I4</f>
+        <v>electric_arc_furnace</v>
+      </c>
+      <c r="B49" s="95" t="str">
+        <f>is_high_temp_process!B4:J4</f>
+        <v>electricity</v>
+      </c>
+      <c r="C49" s="95">
+        <f>is_high_temp_process!C4:K4</f>
+        <v>5.5</v>
+      </c>
+      <c r="D49" s="95">
+        <f>is_high_temp_process!D4:L4</f>
+        <v>5.5</v>
+      </c>
+      <c r="E49" s="95">
+        <f>is_high_temp_process!E4:M4</f>
+        <v>2050</v>
+      </c>
+      <c r="F49" s="95" t="str">
+        <f>is_high_temp_process!F4:N4</f>
+        <v>linear</v>
+      </c>
+      <c r="G49" s="95">
+        <f>is_high_temp_process!G4:O4</f>
+        <v>2010</v>
+      </c>
+      <c r="H49" s="95" t="str">
+        <f>is_high_temp_process!H4:P4</f>
+        <v>steel_production</v>
+      </c>
+      <c r="I49" s="95">
+        <f>is_high_temp_process!I4:Q4</f>
+        <v>1</v>
+      </c>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="95" t="str">
+        <f>is_high_temp_process!A5:I5</f>
+        <v>SNG_furnace</v>
+      </c>
+      <c r="B50" s="95" t="str">
+        <f>is_high_temp_process!B5:J5</f>
+        <v>gas</v>
+      </c>
+      <c r="C50" s="95">
+        <f>is_high_temp_process!C5:K5</f>
+        <v>1</v>
+      </c>
+      <c r="D50" s="95">
+        <f>is_high_temp_process!D5:L5</f>
+        <v>1</v>
+      </c>
+      <c r="E50" s="95">
+        <f>is_high_temp_process!E5:M5</f>
+        <v>2050</v>
+      </c>
+      <c r="F50" s="95" t="str">
+        <f>is_high_temp_process!F5:N5</f>
+        <v>linear</v>
+      </c>
+      <c r="G50" s="95">
+        <f>is_high_temp_process!G5:O5</f>
+        <v>2020</v>
+      </c>
+      <c r="H50" s="95" t="str">
+        <f>is_high_temp_process!H5:P5</f>
+        <v>steel_production</v>
+      </c>
+      <c r="I50" s="95">
+        <f>is_high_temp_process!I5:Q5</f>
+        <v>1</v>
+      </c>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="95" t="str">
+        <f>is_high_temp_process!A6:I6</f>
+        <v>biomass_furnace</v>
+      </c>
+      <c r="B51" s="95" t="str">
+        <f>is_high_temp_process!B6:J6</f>
+        <v>biomass</v>
+      </c>
+      <c r="C51" s="95">
+        <f>is_high_temp_process!C6:K6</f>
+        <v>1</v>
+      </c>
+      <c r="D51" s="95">
+        <f>is_high_temp_process!D6:L6</f>
+        <v>1</v>
+      </c>
+      <c r="E51" s="95">
+        <f>is_high_temp_process!E6:M6</f>
+        <v>2050</v>
+      </c>
+      <c r="F51" s="95" t="str">
+        <f>is_high_temp_process!F6:N6</f>
+        <v>linear</v>
+      </c>
+      <c r="G51" s="95">
+        <f>is_high_temp_process!G6:O6</f>
+        <v>2020</v>
+      </c>
+      <c r="H51" s="95" t="str">
+        <f>is_high_temp_process!H6:P6</f>
+        <v>steel_production</v>
+      </c>
+      <c r="I51" s="95">
+        <f>is_high_temp_process!I6:Q6</f>
+        <v>1</v>
+      </c>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="95" t="str">
+        <f>is_high_temp_process!A7:I7</f>
+        <v>hydrogen_furnace</v>
+      </c>
+      <c r="B52" s="95" t="str">
+        <f>is_high_temp_process!B7:J7</f>
+        <v>hydrogen</v>
+      </c>
+      <c r="C52" s="95">
+        <f>is_high_temp_process!C7:K7</f>
+        <v>1</v>
+      </c>
+      <c r="D52" s="95">
+        <f>is_high_temp_process!D7:L7</f>
+        <v>1</v>
+      </c>
+      <c r="E52" s="95">
+        <f>is_high_temp_process!E7:M7</f>
+        <v>2015</v>
+      </c>
+      <c r="F52" s="95" t="str">
+        <f>is_high_temp_process!F7:N7</f>
+        <v>linear</v>
+      </c>
+      <c r="G52" s="95">
+        <f>is_high_temp_process!G7:O7</f>
+        <v>202</v>
+      </c>
+      <c r="H52" s="95" t="str">
+        <f>is_high_temp_process!H7:P7</f>
+        <v>steel_production</v>
+      </c>
+      <c r="I52" s="95">
+        <f>is_high_temp_process!I7:Q7</f>
+        <v>1</v>
+      </c>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J61" s="5"/>
     </row>
   </sheetData>
@@ -4758,8 +4929,8 @@
     <col min="11" max="11" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:26" s="98" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5030,8 +5201,8 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="17" spans="1:7" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+    <row r="17" spans="1:7" s="99" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
         <v>79</v>
       </c>
     </row>
@@ -5212,8 +5383,8 @@
     <col min="12" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:11" s="98" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5395,8 +5566,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+    <row r="17" spans="1:6" s="99" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
         <v>79</v>
       </c>
     </row>
@@ -6331,18 +6502,18 @@
       <c r="L97" s="2"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A98" s="98" t="s">
+      <c r="A98" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="B98" s="98"/>
-      <c r="C98" s="98"/>
-      <c r="D98" s="98"/>
-      <c r="E98" s="98"/>
-      <c r="F98" s="98"/>
-      <c r="G98" s="98"/>
-      <c r="H98" s="98"/>
-      <c r="I98" s="98"/>
-      <c r="J98" s="98"/>
+      <c r="B98" s="100"/>
+      <c r="C98" s="100"/>
+      <c r="D98" s="100"/>
+      <c r="E98" s="100"/>
+      <c r="F98" s="100"/>
+      <c r="G98" s="100"/>
+      <c r="H98" s="100"/>
+      <c r="I98" s="100"/>
+      <c r="J98" s="100"/>
       <c r="K98" s="47"/>
       <c r="L98" s="38"/>
     </row>
@@ -6434,16 +6605,16 @@
     </row>
     <row r="102" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="105" spans="1:14" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="98" t="s">
+      <c r="A105" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="B105" s="98"/>
-      <c r="C105" s="98"/>
-      <c r="D105" s="98"/>
-      <c r="E105" s="98"/>
-      <c r="F105" s="98"/>
-      <c r="G105" s="98"/>
-      <c r="H105" s="98"/>
+      <c r="B105" s="100"/>
+      <c r="C105" s="100"/>
+      <c r="D105" s="100"/>
+      <c r="E105" s="100"/>
+      <c r="F105" s="100"/>
+      <c r="G105" s="100"/>
+      <c r="H105" s="100"/>
       <c r="I105" s="64"/>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.25">
@@ -6640,8 +6811,8 @@
     <col min="9" max="9" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:12" s="98" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>121</v>
       </c>
     </row>
@@ -7006,8 +7177,8 @@
     <col min="12" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:11" s="98" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>134</v>
       </c>
     </row>
@@ -7190,8 +7361,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+    <row r="17" spans="1:6" s="99" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
         <v>79</v>
       </c>
     </row>
@@ -8868,8 +9039,8 @@
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:10" s="98" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>154</v>
       </c>
     </row>
@@ -9607,8 +9778,8 @@
     <col min="9" max="9" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:10" s="98" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>139</v>
       </c>
     </row>
@@ -9907,8 +10078,8 @@
     <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:10" s="98" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>172</v>
       </c>
     </row>
@@ -10218,8 +10389,8 @@
     <row r="14" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" s="93" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+    <row r="17" spans="1:6" s="99" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
         <v>79</v>
       </c>
     </row>
@@ -10296,7 +10467,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10311,8 +10482,8 @@
     <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="96" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:10" s="98" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="98" t="s">
         <v>172</v>
       </c>
     </row>
@@ -10502,8 +10673,8 @@
     <row r="14" spans="1:10" s="94" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:10" s="94" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:10" s="94" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:6" s="97" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
+    <row r="17" spans="1:6" s="99" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="99" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
before reworking weather regional specfic correction factor
</commit_message>
<xml_diff>
--- a/energy_demand/config_data/05-technologies/efficiency_generation_spreadsheet.xlsx
+++ b/energy_demand/config_data/05-technologies/efficiency_generation_spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="14460" windowHeight="14925"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="14460" windowHeight="14925" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -3343,7 +3343,7 @@
   </sheetPr>
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
@@ -10466,8 +10466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10696,7 +10696,7 @@
         <v>181</v>
       </c>
       <c r="B22">
-        <v>11</v>
+        <v>10.5</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -10707,11 +10707,11 @@
         <v>183</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="C23">
         <f>B22/B23</f>
-        <v>5.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>